<commit_message>
working on qPCR analysis
standard curve works...
working on sample calculations now
</commit_message>
<xml_diff>
--- a/qPCR_CFX/compare.xlsx
+++ b/qPCR_CFX/compare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrouwer\Documents\molecular_tools\qPCR_CFX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A470BC9-654D-4999-A3E4-D414CF24471F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF3B54C-B274-41DD-9D2B-6CF69A7D1C0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="-120" windowWidth="24330" windowHeight="15990" xr2:uid="{D317EC17-2EA7-4B80-9E9E-3FBA3CB98F2B}"/>
+    <workbookView xWindow="990" yWindow="-120" windowWidth="24330" windowHeight="15990" activeTab="1" xr2:uid="{D317EC17-2EA7-4B80-9E9E-3FBA3CB98F2B}"/>
   </bookViews>
   <sheets>
     <sheet name="results 1" sheetId="1" r:id="rId1"/>
@@ -366,7 +366,7 @@
     <numFmt numFmtId="164" formatCode="###0.00;\-###0.00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,6 +412,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -483,7 +489,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -556,6 +562,12 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3586,8 +3598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19311A8-C023-43DF-944E-656E5AD8A8FA}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5386,10 +5398,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{621098FE-51C8-492D-B62A-74660BA8F3FC}">
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5398,7 +5410,7 @@
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -5409,7 +5421,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -5419,8 +5431,10 @@
       <c r="C2">
         <v>16.149999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -5430,8 +5444,11 @@
       <c r="C3">
         <v>16.13</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -5441,8 +5458,11 @@
       <c r="C4">
         <v>16.86</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -5452,8 +5472,11 @@
       <c r="C5">
         <v>16.27</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G5" s="29"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -5463,8 +5486,11 @@
       <c r="C6">
         <v>15.73</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G6" s="29"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -5474,8 +5500,11 @@
       <c r="C7">
         <v>15.52</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G7" s="29"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>102</v>
       </c>
@@ -5485,8 +5514,11 @@
       <c r="C8">
         <v>16.28</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G8" s="29"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>102</v>
       </c>
@@ -5497,7 +5529,7 @@
         <v>15.56</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>75</v>
       </c>
@@ -5507,8 +5539,9 @@
       <c r="C10">
         <v>16.04</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G10" s="29"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -5519,7 +5552,7 @@
         <v>16.059999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>76</v>
       </c>
@@ -5529,8 +5562,9 @@
       <c r="C12">
         <v>14.65</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G12" s="29"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -5541,7 +5575,7 @@
         <v>14.75</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -5551,8 +5585,9 @@
       <c r="C14">
         <v>15.88</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G14" s="29"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -5563,7 +5598,7 @@
         <v>15.61</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -6206,5 +6241,6 @@
     <sortCondition ref="A4:A63"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>